<commit_message>
add network panic for document
</commit_message>
<xml_diff>
--- a/pingfen/collect.xlsx
+++ b/pingfen/collect.xlsx
@@ -4381,7 +4381,7 @@
         <v>25</v>
       </c>
       <c r="NN4" s="17">
-        <v>3071</v>
+        <v>3072</v>
       </c>
       <c r="NO4" s="17">
         <v>7.5</v>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="NM6" s="17"/>
       <c r="NN6" s="17">
-        <v>1454.37</v>
+        <v>1454.64</v>
       </c>
       <c r="NO6" s="17">
         <v>7.8</v>
@@ -9895,7 +9895,7 @@
         <v>3070</v>
       </c>
       <c r="DX13" s="19">
-        <v>3071</v>
+        <v>3072</v>
       </c>
       <c r="DY13" s="19"/>
       <c r="DZ13" s="4" t="s"/>
@@ -15504,7 +15504,7 @@
         <v>253</v>
       </c>
       <c r="DV3" s="37">
-        <v>254.3</v>
+        <v>254.4</v>
       </c>
       <c r="DW3" s="37"/>
       <c r="DX3" s="37"/>

</xml_diff>